<commit_message>
Working with the original data
so fetched the categories and data correctly and priority is implemented.

also that is feteched to the backend and displayed again to the front end..

so brought working connectivity
</commit_message>
<xml_diff>
--- a/Master health check icsa Feb 24.xlsx
+++ b/Master health check icsa Feb 24.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\tester-product\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C67107F-B490-4864-852F-2ED9F3FF823D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CDD9734-BC98-4D83-BECA-967CF3127D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="811" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2473,11 +2473,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K99"/>
+  <dimension ref="A2:K100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2583,329 +2583,326 @@
     <col min="100" max="16384" width="9.33203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H3" s="15" t="s">
         <v>250</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>112</v>
+        <v>297</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>120</v>
+        <v>256</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>258</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>128</v>
+        <v>103</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>104</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>135</v>
+        <v>105</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>160</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>200</v>
+        <v>298</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>176</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>203</v>
+        <v>281</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
     </row>
-    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
@@ -2934,8 +2931,8 @@
     <row r="22" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
     </row>
-    <row r="24" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
+    <row r="23" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
     </row>
     <row r="25" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
@@ -2964,8 +2961,8 @@
     <row r="33" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
     </row>
-    <row r="35" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
+    <row r="34" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
     </row>
     <row r="36" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
@@ -2994,8 +2991,8 @@
     <row r="44" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
     </row>
-    <row r="46" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="2"/>
+    <row r="45" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
     </row>
     <row r="47" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
@@ -3024,8 +3021,8 @@
     <row r="55" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
     </row>
-    <row r="57" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="2"/>
+    <row r="56" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2"/>
     </row>
     <row r="58" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
@@ -3054,8 +3051,8 @@
     <row r="66" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
     </row>
-    <row r="68" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="2"/>
+    <row r="67" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="2"/>
     </row>
     <row r="69" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
@@ -3084,10 +3081,10 @@
     <row r="77" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
     </row>
-    <row r="78" spans="1:1" ht="15.6" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="2"/>
-    </row>
+    <row r="78" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="2"/>
+    </row>
+    <row r="79" spans="1:1" ht="15.6" x14ac:dyDescent="0.25"/>
     <row r="80" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
     </row>
@@ -3115,8 +3112,8 @@
     <row r="88" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
     </row>
-    <row r="90" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="2"/>
+    <row r="89" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="2"/>
     </row>
     <row r="91" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
@@ -3144,6 +3141,9 @@
     </row>
     <row r="99" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
+    </row>
+    <row r="100" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6635,6 +6635,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100ED5DB048F347B545B3F3002901E87BC2" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0d5f6051fe61e0fab499ca941bb355b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5ea14ac2-ef12-443e-9168-5089afbf69bd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ed229c097dffbb4490c98383a4edc4ce" ns3:_="">
     <xsd:import namespace="5ea14ac2-ef12-443e-9168-5089afbf69bd"/>
@@ -6810,15 +6819,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DA2FA42-43A6-4B13-A92B-32543A09ED51}">
   <ds:schemaRefs>
@@ -6836,6 +6836,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D829BA9C-9853-4626-9E7D-A3A36F005C8A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E365D55F-915F-4D57-BBA9-32D41FED17B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6851,12 +6859,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D829BA9C-9853-4626-9E7D-A3A36F005C8A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated on the criteria fetching
</commit_message>
<xml_diff>
--- a/Master health check icsa Feb 24.xlsx
+++ b/Master health check icsa Feb 24.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\tester-product\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CDD9734-BC98-4D83-BECA-967CF3127D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0797DC48-68E9-4565-A0BC-966FC253955C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="811" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="811" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="4" r:id="rId1"/>
-    <sheet name="Cash KPIs" sheetId="16" r:id="rId2"/>
+    <sheet name="metrics" sheetId="16" r:id="rId2"/>
     <sheet name="SaaS KPIs" sheetId="6" r:id="rId3"/>
     <sheet name="Inventory KPIs" sheetId="19" r:id="rId4"/>
     <sheet name="Investors KPIs" sheetId="20" r:id="rId5"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="494">
   <si>
     <t>Return on Equity</t>
   </si>
@@ -1516,6 +1516,12 @@
   </si>
   <si>
     <t>Temporary workers time</t>
+  </si>
+  <si>
+    <t>OTHER KPIs</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -2473,11 +2479,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:K100"/>
+  <dimension ref="A2:AB100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2583,7 +2589,7 @@
     <col min="100" max="16384" width="9.33203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
@@ -2618,7 +2624,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>41</v>
       </c>
@@ -2653,7 +2659,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>296</v>
       </c>
@@ -2688,7 +2694,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>297</v>
       </c>
@@ -2723,7 +2729,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>112</v>
       </c>
@@ -2758,7 +2764,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>138</v>
       </c>
@@ -2793,7 +2799,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>298</v>
       </c>
@@ -2828,7 +2834,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>179</v>
       </c>
@@ -2863,7 +2869,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>204</v>
       </c>
@@ -2898,19 +2904,63 @@
         <v>294</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="U11" s="11"/>
+      <c r="V11" s="3"/>
+      <c r="X11" s="11"/>
+      <c r="Y11" s="11"/>
+      <c r="AA11" s="11"/>
+      <c r="AB11" s="11"/>
+    </row>
+    <row r="12" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
     </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3156,8 +3206,8 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3494,11 +3544,11 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="86" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3539,319 +3589,228 @@
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>2</v>
+      </c>
       <c r="D2" s="20" t="s">
         <v>309</v>
       </c>
       <c r="E2" s="19" t="s">
         <v>481</v>
       </c>
-      <c r="F2" s="19"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="29" t="e">
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
     </row>
     <row r="3" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>0</v>
+      <c r="A3" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
+        <v>5</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>386</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>387</v>
+      </c>
       <c r="F3" s="17"/>
       <c r="G3" s="29" t="e">
-        <f>D3/E3</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C4" s="6"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>482</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>481</v>
+      </c>
+      <c r="F4" s="17"/>
+      <c r="G4" s="29" t="e">
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="D5" s="20" t="s">
-        <v>386</v>
+        <v>483</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>387</v>
-      </c>
-      <c r="F5" s="19"/>
+        <v>484</v>
+      </c>
+      <c r="F5" s="17"/>
+      <c r="G5" s="29" t="e">
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>3</v>
+      <c r="A6" s="12" t="s">
+        <v>230</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="17"/>
+        <v>12</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>445</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>446</v>
+      </c>
       <c r="F6" s="17"/>
       <c r="G6" s="29" t="e">
-        <f>D6/E6</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="11"/>
-      <c r="C7" s="9"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>389</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>390</v>
+      </c>
+      <c r="F7" s="17"/>
+      <c r="G7" s="29" t="e">
+        <f>(#REF!-#REF!)/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>17</v>
+      </c>
       <c r="D8" s="20" t="s">
-        <v>482</v>
+        <v>309</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>481</v>
-      </c>
-      <c r="F8" s="19"/>
+        <v>389</v>
+      </c>
+      <c r="F8" s="17"/>
+      <c r="G8" s="29" t="e">
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>6</v>
+        <v>232</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
+        <v>231</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>485</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>486</v>
+      </c>
       <c r="F9" s="17"/>
       <c r="G9" s="29" t="e">
-        <f>D9/E9</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="11"/>
-      <c r="D10" s="9"/>
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>389</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>463</v>
+      </c>
+      <c r="F10" s="17"/>
+      <c r="G10" s="29" t="e">
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
+      <c r="A11" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>22</v>
+      </c>
       <c r="D11" s="20" t="s">
-        <v>483</v>
+        <v>390</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>484</v>
-      </c>
-      <c r="F11" s="19"/>
-    </row>
-    <row r="12" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
-        <v>229</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="29" t="e">
-        <f>D12/E12</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="11"/>
-    </row>
-    <row r="14" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="D14" s="20" t="s">
-        <v>445</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>446</v>
-      </c>
-      <c r="F14" s="19"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
-        <v>230</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="29" t="e">
-        <f>D15/E15</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="11"/>
-      <c r="C16" s="9"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D17" s="20" t="s">
-        <v>389</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>390</v>
-      </c>
-      <c r="F17" s="19"/>
-    </row>
-    <row r="18" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
-        <v>295</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="29" t="e">
-        <f>(D18-E18)/D18</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="11"/>
-      <c r="D19" s="9"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="20" t="s">
-        <v>309</v>
-      </c>
-      <c r="E20" s="19" t="s">
-        <v>389</v>
-      </c>
-      <c r="F20" s="19"/>
-    </row>
-    <row r="21" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="29" t="e">
-        <f>D21/E21</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="11"/>
-    </row>
-    <row r="23" spans="1:8" s="3" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="D23" s="20" t="s">
-        <v>485</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>486</v>
-      </c>
-      <c r="F23" s="19"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="4"/>
-    </row>
-    <row r="24" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>231</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>233</v>
-      </c>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="29" t="e">
-        <f>D24/E24</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="11"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D26" s="20" t="s">
-        <v>389</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>463</v>
-      </c>
-      <c r="F26" s="19"/>
-    </row>
-    <row r="27" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="29" t="e">
-        <f>D27/E27</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="11"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D29" s="20" t="s">
-        <v>390</v>
-      </c>
-      <c r="E29" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="F29" s="19"/>
-    </row>
-    <row r="30" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="29" t="e">
-        <f>D30/E30</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="11"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="29" t="e">
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3861,26 +3820,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:J101"/>
   <sheetViews>
-    <sheetView zoomScale="91" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="57" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G101" sqref="G101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="35.21875" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.44140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="47.33203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.77734375" style="11" customWidth="1"/>
-    <col min="6" max="6" width="23.6640625" style="11" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" style="21" customWidth="1"/>
-    <col min="8" max="16384" width="9.33203125" style="4"/>
+    <col min="3" max="3" width="47.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.33203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>299</v>
       </c>
@@ -3900,303 +3862,3005 @@
         <v>316</v>
       </c>
       <c r="G1" s="27" t="s">
+        <v>342</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>358</v>
+      </c>
+      <c r="I1" s="27" t="s">
         <v>304</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="J1" s="27" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>487</v>
+      </c>
       <c r="D2" s="19" t="s">
         <v>302</v>
       </c>
       <c r="E2" s="19" t="s">
         <v>303</v>
       </c>
-      <c r="F2" s="19"/>
-    </row>
-    <row r="3" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>235</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>487</v>
-      </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="29">
+      <c r="F2" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I2" s="29" t="e">
+        <f>D2-E2</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>307</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>308</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I3" s="29" t="e">
         <f>D3-E3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>309</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>310</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>488</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I4" s="29" t="e">
+        <f>D4+E4-F4</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="D5" s="19" t="s">
+        <v>311</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>312</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>313</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I5" s="29" t="e">
+        <f>D5+E5-F5</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>317</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>318</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I6" s="29" t="str">
+        <f>IFERROR(D6/E6,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>319</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I7" s="29" t="str">
+        <f>IFERROR((D7/E7)*365,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>320</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I8" s="29" t="str">
+        <f>IFERROR((D8/E8)*365,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>322</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>323</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I9" s="29" t="str">
+        <f>IFERROR((D9/E9)*365,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>324</v>
+      </c>
+      <c r="E10" s="19" t="s">
         <v>307</v>
       </c>
-      <c r="E5" s="19" t="s">
-        <v>308</v>
-      </c>
-      <c r="F5" s="19"/>
-    </row>
-    <row r="6" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>236</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>306</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="29">
-        <f>D6-E6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D8" s="20" t="s">
-        <v>309</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>310</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>238</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="29">
-        <f>D9+E9-F9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="D11" s="19" t="s">
-        <v>311</v>
+      <c r="F10" s="19" t="s">
+        <v>325</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I10" s="29" t="e">
+        <f>D10+E10-F10</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>326</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>312</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
-        <v>239</v>
+        <v>327</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I11" s="29" t="str">
+        <f>IFERROR(D11/E11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>246</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="29">
-        <f>D12+E12-F12</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>328</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>329</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I12" s="29" t="str">
+        <f>IFERROR(D12/E12,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>330</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>331</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I13" s="29" t="str">
+        <f>IFERROR((D13-E13)/E13,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="D14" s="20" t="s">
-        <v>317</v>
+        <v>332</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>318</v>
-      </c>
-      <c r="F14" s="19"/>
-    </row>
-    <row r="15" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
-        <v>29</v>
+        <v>333</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I14" s="29" t="e">
+        <f>D14*E14</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>248</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="29" t="str">
+        <v>50</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>334</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>335</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I15" s="29" t="str">
         <f>IFERROR(D15/E15,"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>336</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>337</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H16" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I16" s="29" t="str">
+        <f>IFERROR(D16/E16,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="D17" s="20" t="s">
+        <v>338</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>339</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I17" s="29" t="str">
+        <f>IFERROR(D17/E17,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>340</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>341</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H18" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I18" s="29" t="str">
+        <f>IFERROR(D18/E18,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>346</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>343</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>345</v>
+      </c>
+      <c r="G19" s="21" t="s">
+        <v>344</v>
+      </c>
+      <c r="I19" s="29" t="e">
+        <f>(D19+E19)/(F19+G19)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>347</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>348</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I20" s="29" t="e">
+        <f>D20*E20</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>349</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I21" s="29" t="e">
+        <f>D21*E21</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="E17" s="19" t="s">
-        <v>319</v>
-      </c>
-      <c r="F17" s="19"/>
-    </row>
-    <row r="18" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
-        <v>240</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>241</v>
-      </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="29" t="str">
-        <f>IFERROR((D18/E18)*365,"")</f>
+      <c r="B22" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>351</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>352</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I22" s="29" t="str">
+        <f>IFERROR((D22+E22)/2,"")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="D20" s="19" t="s">
-        <v>320</v>
-      </c>
-      <c r="E20" s="19" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
-        <v>242</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="29" t="str">
-        <f>IFERROR((D21/E21)*365,"")</f>
+    <row r="23" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>353</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>354</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I23" s="29" t="str">
+        <f>IFERROR((D23/E23)*365,"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="D23" s="20" t="s">
-        <v>322</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>323</v>
-      </c>
-      <c r="F23" s="19"/>
-    </row>
-    <row r="24" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>243</v>
+        <v>254</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="29" t="str">
-        <f>IFERROR((D24/E24)*365,"")</f>
+        <v>71</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>355</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>356</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G24" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I24" s="29" t="e">
+        <f>D24/E24</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>361</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>362</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>360</v>
+      </c>
+      <c r="G25" s="19" t="s">
+        <v>359</v>
+      </c>
+      <c r="H25" s="19" t="s">
+        <v>357</v>
+      </c>
+      <c r="I25" s="29" t="e">
+        <f>(D25+E25+F25+G25)/H25</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="20" t="s">
+        <v>364</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>363</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G26" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H26" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I26" s="29" t="str">
+        <f>IFERROR(D26/E26,"")</f>
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D26" s="19" t="s">
-        <v>324</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>307</v>
-      </c>
-      <c r="F26" s="19" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
-        <v>244</v>
+    <row r="27" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>77</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>37</v>
+        <v>78</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="29">
-        <f>D27+E27-F27</f>
+        <v>79</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>365</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>366</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G27" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H27" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I27" s="29" t="str">
+        <f>IFERROR(D27/E27,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>367</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>368</v>
+      </c>
+      <c r="F28" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G28" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H28" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I28" s="29" t="str">
+        <f>IFERROR(D28/E28,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>370</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>371</v>
+      </c>
+      <c r="F29" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="G29" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H29" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I29" s="29" t="e">
+        <f>D29+E29+F29</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>372</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>373</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G30" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H30" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I30" s="29" t="e">
+        <f>D30-E30</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>375</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>376</v>
+      </c>
+      <c r="F31" s="19" t="s">
+        <v>374</v>
+      </c>
+      <c r="G31" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H31" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I31" s="29" t="e">
+        <f>D31+E31-F31</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>377</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>378</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G32" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H32" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I32" s="29" t="str">
+        <f t="shared" ref="I32:I38" si="0">IFERROR(D32/E32,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>379</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>380</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G33" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H33" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I33" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>309</v>
+      </c>
+      <c r="E34" s="20" t="s">
+        <v>381</v>
+      </c>
+      <c r="F34" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G34" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H34" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I34" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>257</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G35" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H35" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I35" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A36" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>383</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="F36" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G36" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H36" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I36" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>384</v>
+      </c>
+      <c r="E37" s="20" t="s">
+        <v>385</v>
+      </c>
+      <c r="F37" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G37" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H37" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I37" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="20" t="s">
+        <v>386</v>
+      </c>
+      <c r="E38" s="20" t="s">
+        <v>387</v>
+      </c>
+      <c r="F38" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G38" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H38" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I38" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D39" s="20" t="s">
+        <v>386</v>
+      </c>
+      <c r="E39" s="20" t="s">
+        <v>388</v>
+      </c>
+      <c r="F39" s="20" t="s">
+        <v>387</v>
+      </c>
+      <c r="G39" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H39" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I39" s="29" t="str">
+        <f>IFERROR((D39-E39)/F39,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>389</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>390</v>
+      </c>
+      <c r="F40" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G40" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H40" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I40" s="29" t="str">
+        <f>IFERROR((D40-E40)/D40,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A41" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>391</v>
+      </c>
+      <c r="E41" s="20" t="s">
+        <v>392</v>
+      </c>
+      <c r="F41" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G41" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H41" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I41" s="29" t="e">
+        <f>D41-E41</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A42" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>393</v>
+      </c>
+      <c r="E42" s="20" t="s">
+        <v>394</v>
+      </c>
+      <c r="F42" s="18" t="s">
+        <v>493</v>
+      </c>
+      <c r="G42" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H42" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I42" s="31" t="e">
+        <f>D42+E42</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A43" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="D43" s="20" t="s">
+        <v>395</v>
+      </c>
+      <c r="E43" s="20" t="s">
+        <v>396</v>
+      </c>
+      <c r="F43" s="18" t="s">
+        <v>493</v>
+      </c>
+      <c r="G43" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H43" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I43" s="31" t="str">
+        <f>IFERROR(D43/E43,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D44" s="20" t="s">
+        <v>397</v>
+      </c>
+      <c r="E44" s="20" t="s">
+        <v>398</v>
+      </c>
+      <c r="F44" s="18" t="s">
+        <v>493</v>
+      </c>
+      <c r="G44" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H44" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I44" s="31" t="str">
+        <f>IFERROR(D44/E44,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D45" s="20" t="s">
+        <v>399</v>
+      </c>
+      <c r="E45" s="20" t="s">
+        <v>400</v>
+      </c>
+      <c r="F45" s="18" t="s">
+        <v>493</v>
+      </c>
+      <c r="G45" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H45" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I45" s="31" t="e">
+        <f>D45+E45</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A46" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>401</v>
+      </c>
+      <c r="E46" s="20" t="s">
+        <v>402</v>
+      </c>
+      <c r="F46" s="18" t="s">
+        <v>493</v>
+      </c>
+      <c r="G46" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H46" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I46" s="31" t="e">
+        <f>D46*E46</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A47" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="D47" s="20" t="s">
+        <v>405</v>
+      </c>
+      <c r="E47" s="20" t="s">
+        <v>404</v>
+      </c>
+      <c r="F47" s="20" t="s">
+        <v>403</v>
+      </c>
+      <c r="G47" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H47" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I47" s="31" t="e">
+        <f>D47+E47+F47</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A48" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="D48" s="20" t="s">
+        <v>489</v>
+      </c>
+      <c r="E48" s="20" t="s">
+        <v>490</v>
+      </c>
+      <c r="F48" s="20" t="s">
+        <v>491</v>
+      </c>
+      <c r="G48" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H48" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I48" s="31"/>
+    </row>
+    <row r="49" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A49" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D49" s="20" t="s">
+        <v>407</v>
+      </c>
+      <c r="E49" s="20" t="s">
+        <v>408</v>
+      </c>
+      <c r="F49" s="20" t="s">
+        <v>406</v>
+      </c>
+      <c r="G49" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H49" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I49" s="31" t="str">
+        <f>IFERROR((D49-E49)/F49,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D50" s="20" t="s">
+        <v>409</v>
+      </c>
+      <c r="E50" s="20" t="s">
+        <v>410</v>
+      </c>
+      <c r="F50" s="18" t="s">
+        <v>493</v>
+      </c>
+      <c r="G50" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H50" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I50" s="31" t="e">
+        <f>D50/E50</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="66" x14ac:dyDescent="0.25">
+      <c r="A51" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D51" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="E51" s="18" t="s">
+        <v>493</v>
+      </c>
+      <c r="F51" s="18" t="s">
+        <v>493</v>
+      </c>
+      <c r="G51" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H51" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I51" s="31" t="str">
+        <f>D51</f>
+        <v>Average number of days between job opening and contract signed by candidate</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="D52" s="20" t="s">
+        <v>411</v>
+      </c>
+      <c r="E52" s="20" t="s">
+        <v>412</v>
+      </c>
+      <c r="F52" s="18" t="s">
+        <v>493</v>
+      </c>
+      <c r="G52" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H52" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I52" s="32" t="e">
+        <f>D52+E52</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A53" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="D53" s="20" t="s">
+        <v>413</v>
+      </c>
+      <c r="E53" s="20" t="s">
+        <v>414</v>
+      </c>
+      <c r="F53" s="18" t="s">
+        <v>493</v>
+      </c>
+      <c r="G53" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H53" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I53" s="32" t="e">
+        <f>D53/E53</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="D54" s="20" t="s">
+        <v>389</v>
+      </c>
+      <c r="E54" s="20" t="s">
+        <v>415</v>
+      </c>
+      <c r="F54" s="18" t="s">
+        <v>493</v>
+      </c>
+      <c r="G54" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H54" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I54" s="32" t="e">
+        <f>D54/E54</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A55" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D55" s="20" t="s">
+        <v>309</v>
+      </c>
+      <c r="E55" s="20" t="s">
+        <v>416</v>
+      </c>
+      <c r="F55" s="18" t="s">
+        <v>493</v>
+      </c>
+      <c r="G55" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H55" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I55" s="32" t="e">
+        <f>D55/E55</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A56" s="12" t="s">
+        <v>270</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="D56" s="20" t="s">
+        <v>417</v>
+      </c>
+      <c r="E56" s="20" t="s">
+        <v>418</v>
+      </c>
+      <c r="F56" s="18" t="s">
+        <v>493</v>
+      </c>
+      <c r="G56" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H56" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I56" s="32" t="e">
+        <f>D56/E56</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D57" s="20" t="s">
+        <v>419</v>
+      </c>
+      <c r="E57" s="20" t="s">
+        <v>420</v>
+      </c>
+      <c r="F57" s="18" t="s">
+        <v>493</v>
+      </c>
+      <c r="G57" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H57" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I57" s="32" t="e">
+        <f>D57/E57</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A58" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="D58" s="20" t="s">
+        <v>422</v>
+      </c>
+      <c r="E58" s="20" t="s">
+        <v>423</v>
+      </c>
+      <c r="F58" s="20" t="s">
+        <v>421</v>
+      </c>
+      <c r="G58" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H58" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I58" s="32" t="e">
+        <f>((D58-E58)^((1/F58)-1))</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A59" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="D59" s="20" t="s">
+        <v>425</v>
+      </c>
+      <c r="E59" s="20" t="s">
+        <v>426</v>
+      </c>
+      <c r="F59" s="20" t="s">
+        <v>424</v>
+      </c>
+      <c r="G59" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H59" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I59" s="32" t="e">
+        <f>(D59/((1+E59)^F59))</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="D60" s="20" t="s">
+        <v>266</v>
+      </c>
+      <c r="E60" s="20" t="s">
+        <v>427</v>
+      </c>
+      <c r="F60" s="18" t="s">
+        <v>493</v>
+      </c>
+      <c r="G60" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H60" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I60" s="32" t="e">
+        <f>D60/E60</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="D61" s="20" t="s">
+        <v>428</v>
+      </c>
+      <c r="E61" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="F61" s="18" t="s">
+        <v>493</v>
+      </c>
+      <c r="G61" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H61" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I61" s="32" t="e">
+        <f>D61*E61*100%</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A62" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>273</v>
+      </c>
+      <c r="D62" s="20" t="s">
+        <v>430</v>
+      </c>
+      <c r="E62" s="19" t="s">
+        <v>431</v>
+      </c>
+      <c r="F62" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G62" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H62" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I62" s="29" t="e">
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A63" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="D63" s="20" t="s">
+        <v>432</v>
+      </c>
+      <c r="E63" s="19" t="s">
+        <v>433</v>
+      </c>
+      <c r="F63" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G63" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H63" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I63" s="29" t="e">
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A64" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="D64" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="E64" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="F64" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G64" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H64" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I64" s="29"/>
+    </row>
+    <row r="65" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A65" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="D65" s="20" t="s">
+        <v>416</v>
+      </c>
+      <c r="E65" s="19" t="s">
+        <v>435</v>
+      </c>
+      <c r="F65" s="19" t="s">
+        <v>434</v>
+      </c>
+      <c r="G65" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H65" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I65" s="29" t="e">
+        <f>(#REF!-#REF!)/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A66" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="D66" s="20" t="s">
+        <v>436</v>
+      </c>
+      <c r="E66" s="19" t="s">
+        <v>437</v>
+      </c>
+      <c r="F66" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G66" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H66" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I66" s="29" t="e">
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A67" s="12" t="s">
+        <v>278</v>
+      </c>
+      <c r="B67" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="C67" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="D67" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="E67" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="F67" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G67" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H67" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I67" s="29"/>
+    </row>
+    <row r="68" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A68" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="D68" s="20" t="s">
+        <v>438</v>
+      </c>
+      <c r="E68" s="19" t="s">
+        <v>439</v>
+      </c>
+      <c r="F68" s="19" t="s">
+        <v>440</v>
+      </c>
+      <c r="G68" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H68" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I68" s="29" t="e">
+        <f>#REF!/(#REF!+#REF!)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A69" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="D69" s="20" t="s">
+        <v>416</v>
+      </c>
+      <c r="E69" s="19" t="s">
+        <v>435</v>
+      </c>
+      <c r="F69" s="19" t="s">
+        <v>441</v>
+      </c>
+      <c r="G69" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H69" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I69" s="29" t="e">
+        <f>#REF!-#REF!-#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A70" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="D70" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="E70" s="19" t="s">
+        <v>442</v>
+      </c>
+      <c r="F70" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G70" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H70" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I70" s="29" t="e">
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A71" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="D71" s="20" t="s">
+        <v>443</v>
+      </c>
+      <c r="E71" s="19" t="s">
+        <v>416</v>
+      </c>
+      <c r="F71" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G71" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H71" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I71" s="29" t="e">
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A72" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="D72" s="20" t="s">
+        <v>444</v>
+      </c>
+      <c r="E72" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="F72" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G72" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H72" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I72" s="29" t="e">
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A73" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="B73" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D73" s="20" t="s">
+        <v>445</v>
+      </c>
+      <c r="E73" s="19" t="s">
+        <v>446</v>
+      </c>
+      <c r="F73" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G73" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H73" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I73" s="29" t="e">
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A74" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="B74" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="D74" s="20" t="s">
+        <v>447</v>
+      </c>
+      <c r="E74" s="19" t="s">
+        <v>448</v>
+      </c>
+      <c r="F74" s="19" t="s">
+        <v>449</v>
+      </c>
+      <c r="G74" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H74" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I74" s="29" t="e">
+        <f>#REF!-#REF!-#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A75" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="D75" s="20" t="s">
+        <v>450</v>
+      </c>
+      <c r="E75" s="19" t="s">
+        <v>451</v>
+      </c>
+      <c r="F75" s="19" t="s">
+        <v>452</v>
+      </c>
+      <c r="G75" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H75" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I75" s="29" t="e">
+        <f>(#REF!+#REF!)/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A76" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="C76" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="D76" s="20" t="s">
+        <v>453</v>
+      </c>
+      <c r="E76" s="19" t="s">
+        <v>454</v>
+      </c>
+      <c r="F76" s="19" t="s">
+        <v>455</v>
+      </c>
+      <c r="G76" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H76" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I76" s="29" t="e">
+        <f>(#REF!-#REF!)*#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A77" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="C77" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="D77" s="20" t="s">
+        <v>456</v>
+      </c>
+      <c r="E77" s="19" t="s">
+        <v>457</v>
+      </c>
+      <c r="F77" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G77" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H77" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I77" s="29" t="e">
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A78" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="B78" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="C78" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D78" s="20" t="s">
+        <v>458</v>
+      </c>
+      <c r="E78" s="19" t="s">
+        <v>457</v>
+      </c>
+      <c r="F78" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G78" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H78" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I78" s="29" t="e">
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A79" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="B79" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="C79" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="D79" s="20" t="s">
+        <v>459</v>
+      </c>
+      <c r="E79" s="19" t="s">
+        <v>460</v>
+      </c>
+      <c r="F79" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G79" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H79" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I79" s="29" t="e">
+        <f>#REF!-#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="C80" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="D80" s="20" t="s">
+        <v>461</v>
+      </c>
+      <c r="E80" s="19" t="s">
+        <v>462</v>
+      </c>
+      <c r="F80" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G80" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H80" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I80" s="29" t="e">
+        <f>#REF!-#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A81" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="B81" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C81" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D81" s="20" t="s">
+        <v>389</v>
+      </c>
+      <c r="E81" s="19" t="s">
+        <v>463</v>
+      </c>
+      <c r="F81" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G81" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H81" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I81" s="29" t="e">
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A82" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="C82" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="D82" s="20" t="s">
+        <v>465</v>
+      </c>
+      <c r="E82" s="19" t="s">
+        <v>464</v>
+      </c>
+      <c r="F82" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G82" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H82" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I82" s="29" t="e">
+        <f>(#REF!-#REF!)/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A83" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="C83" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="D83" s="20" t="s">
+        <v>466</v>
+      </c>
+      <c r="E83" s="19" t="s">
+        <v>467</v>
+      </c>
+      <c r="F83" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G83" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H83" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I83" s="29" t="e">
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A84" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="C84" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="D84" s="20" t="s">
+        <v>468</v>
+      </c>
+      <c r="E84" s="19" t="s">
+        <v>469</v>
+      </c>
+      <c r="F84" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G84" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H84" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I84" s="29" t="e">
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A85" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="B85" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="C85" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="D85" s="20" t="s">
+        <v>470</v>
+      </c>
+      <c r="E85" s="19" t="s">
+        <v>397</v>
+      </c>
+      <c r="F85" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G85" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H85" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I85" s="29" t="e">
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A86" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="C86" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="D86" s="20" t="s">
+        <v>471</v>
+      </c>
+      <c r="E86" s="19" t="s">
+        <v>472</v>
+      </c>
+      <c r="F86" s="19" t="s">
+        <v>473</v>
+      </c>
+      <c r="G86" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H86" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I86" s="29" t="e">
+        <f>#REF!*#REF!*#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A87" s="12" t="s">
+        <v>289</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="C87" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="D87" s="20" t="s">
+        <v>474</v>
+      </c>
+      <c r="E87" s="19" t="s">
+        <v>397</v>
+      </c>
+      <c r="F87" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G87" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H87" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I87" s="29" t="e">
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A88" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="B88" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C88" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="D88" s="20" t="s">
+        <v>475</v>
+      </c>
+      <c r="E88" s="19" t="s">
+        <v>476</v>
+      </c>
+      <c r="F88" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G88" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H88" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I88" s="29" t="e">
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="92.4" x14ac:dyDescent="0.25">
+      <c r="A89" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="B89" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C89" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="D89" s="20" t="s">
+        <v>293</v>
+      </c>
+      <c r="E89" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="F89" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G89" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H89" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I89" s="29" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A90" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="C90" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="D90" s="20" t="s">
+        <v>477</v>
+      </c>
+      <c r="E90" s="19" t="s">
+        <v>478</v>
+      </c>
+      <c r="F90" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G90" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H90" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I90" s="29" t="e">
+        <f>(#REF!/#REF!)*100</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A91" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="B91" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C91" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D91" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="E91" s="19" t="s">
+        <v>480</v>
+      </c>
+      <c r="F91" s="19" t="s">
+        <v>479</v>
+      </c>
+      <c r="G91" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H91" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I91" s="29" t="e">
+        <f>#REF!+#REF!+#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A92" s="12" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D29" s="20" t="s">
-        <v>326</v>
-      </c>
-      <c r="E29" s="19" t="s">
-        <v>327</v>
-      </c>
-      <c r="F29" s="19"/>
-    </row>
-    <row r="30" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="29" t="str">
-        <f>IFERROR(D30/E30,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="9"/>
+      <c r="B92" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C92" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D92" s="20" t="s">
+        <v>309</v>
+      </c>
+      <c r="E92" s="19" t="s">
+        <v>481</v>
+      </c>
+      <c r="F92" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G92" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H92" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I92" s="29" t="e">
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A93" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B93" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C93" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D93" s="20" t="s">
+        <v>386</v>
+      </c>
+      <c r="E93" s="19" t="s">
+        <v>387</v>
+      </c>
+      <c r="F93" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G93" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H93" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I93" s="29" t="e">
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A94" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B94" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C94" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D94" s="20" t="s">
+        <v>482</v>
+      </c>
+      <c r="E94" s="19" t="s">
+        <v>481</v>
+      </c>
+      <c r="F94" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G94" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H94" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I94" s="29" t="e">
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A95" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="B95" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C95" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D95" s="20" t="s">
+        <v>483</v>
+      </c>
+      <c r="E95" s="19" t="s">
+        <v>484</v>
+      </c>
+      <c r="F95" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G95" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H95" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I95" s="29" t="e">
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A96" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="B96" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C96" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D96" s="20" t="s">
+        <v>445</v>
+      </c>
+      <c r="E96" s="19" t="s">
+        <v>446</v>
+      </c>
+      <c r="F96" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G96" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H96" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I96" s="29" t="e">
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A97" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="B97" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C97" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D97" s="20" t="s">
+        <v>389</v>
+      </c>
+      <c r="E97" s="19" t="s">
+        <v>390</v>
+      </c>
+      <c r="F97" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G97" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H97" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I97" s="29" t="e">
+        <f>(#REF!-#REF!)/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A98" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B98" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C98" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D98" s="20" t="s">
+        <v>309</v>
+      </c>
+      <c r="E98" s="19" t="s">
+        <v>389</v>
+      </c>
+      <c r="F98" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G98" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H98" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I98" s="29" t="e">
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A99" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="B99" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="C99" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="D99" s="20" t="s">
+        <v>485</v>
+      </c>
+      <c r="E99" s="19" t="s">
+        <v>486</v>
+      </c>
+      <c r="F99" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G99" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H99" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I99" s="29" t="e">
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A100" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="B100" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C100" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D100" s="20" t="s">
+        <v>389</v>
+      </c>
+      <c r="E100" s="19" t="s">
+        <v>463</v>
+      </c>
+      <c r="F100" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G100" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H100" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I100" s="29" t="e">
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A101" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B101" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C101" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D101" s="20" t="s">
+        <v>390</v>
+      </c>
+      <c r="E101" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="F101" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="G101" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="H101" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="I101" s="29" t="e">
+        <f>#REF!/#REF!</f>
+        <v>#REF!</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4208,9 +6872,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4574,9 +7238,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4962,7 +7626,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5285,8 +7949,8 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5613,8 +8277,8 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5953,8 +8617,8 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6285,7 +8949,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6576,7 +9240,7 @@
       </c>
       <c r="F26" s="19"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>200</v>
       </c>

</xml_diff>

<commit_message>
worked with the css on the results page
</commit_message>
<xml_diff>
--- a/Master health check icsa Feb 24.xlsx
+++ b/Master health check icsa Feb 24.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\tester-product\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0797DC48-68E9-4565-A0BC-966FC253955C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7867E1-DB5F-44C8-9656-53B33FA314A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="811" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="811" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="4" r:id="rId1"/>
@@ -2479,11 +2479,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:AB100"/>
+  <dimension ref="A2:AB99"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2951,8 +2951,8 @@
       <c r="AA11" s="11"/>
       <c r="AB11" s="11"/>
     </row>
-    <row r="12" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+    <row r="13" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
     </row>
     <row r="14" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
@@ -2981,8 +2981,8 @@
     <row r="22" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
     </row>
-    <row r="23" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
+    <row r="24" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
     </row>
     <row r="25" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
@@ -3011,8 +3011,8 @@
     <row r="33" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
     </row>
-    <row r="34" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
+    <row r="35" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
     </row>
     <row r="36" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
@@ -3041,8 +3041,8 @@
     <row r="44" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
     </row>
-    <row r="45" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
+    <row r="46" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
     </row>
     <row r="47" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
@@ -3071,8 +3071,8 @@
     <row r="55" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
     </row>
-    <row r="56" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="2"/>
+    <row r="57" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="2"/>
     </row>
     <row r="58" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
@@ -3101,8 +3101,8 @@
     <row r="66" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
     </row>
-    <row r="67" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="2"/>
+    <row r="68" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="2"/>
     </row>
     <row r="69" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
@@ -3131,10 +3131,10 @@
     <row r="77" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
     </row>
-    <row r="78" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="2"/>
-    </row>
-    <row r="79" spans="1:1" ht="15.6" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="1:1" ht="15.6" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="2"/>
+    </row>
     <row r="80" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
     </row>
@@ -3162,8 +3162,8 @@
     <row r="88" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
     </row>
-    <row r="89" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="2"/>
+    <row r="90" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="2"/>
     </row>
     <row r="91" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
@@ -3191,9 +3191,6 @@
     </row>
     <row r="99" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
-    </row>
-    <row r="100" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3822,8 +3819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="57" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="69" zoomScaleNormal="57" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G101" sqref="G101"/>
     </sheetView>
   </sheetViews>
@@ -5398,7 +5395,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
         <v>267</v>
       </c>
@@ -5488,7 +5485,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
         <v>270</v>
       </c>
@@ -9240,7 +9237,7 @@
       </c>
       <c r="F26" s="19"/>
     </row>
-    <row r="27" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>200</v>
       </c>

</xml_diff>